<commit_message>
History test of GeoBrevet App
</commit_message>
<xml_diff>
--- a/Error_codes.xlsx
+++ b/Error_codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\WampServer\www\learningCenter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9088B557-43AA-4349-BB61-B26C74AE0634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8AF8E2-02F8-4E2A-805B-D6B3687F79E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{63368EE7-2865-4327-9FAE-68BBA3F8F765}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Code</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Message</t>
   </si>
   <si>
-    <t>#2000</t>
-  </si>
-  <si>
     <t>Application inconnue.</t>
   </si>
   <si>
@@ -51,28 +48,53 @@
     <t>Classe</t>
   </si>
   <si>
+    <t>Contenu de l'application inacessible.</t>
+  </si>
+  <si>
+    <t>#1001</t>
+  </si>
+  <si>
+    <t>Historique des versions introuvable.</t>
+  </si>
+  <si>
+    <t>Versions
+#2</t>
+  </si>
+  <si>
     <t>Application
-#2</t>
-  </si>
-  <si>
-    <t>Contenu de l'application inacessible.</t>
-  </si>
-  <si>
-    <t>#1001</t>
-  </si>
-  <si>
-    <t>Versions
+#3</t>
+  </si>
+  <si>
+    <t>#3001</t>
+  </si>
+  <si>
+    <t>Non trouvé
 #1</t>
   </si>
   <si>
-    <t>Historique des versions introuvable.</t>
+    <t>#1000</t>
+  </si>
+  <si>
+    <t>Fichier non trouvé.</t>
+  </si>
+  <si>
+    <t>#3002</t>
+  </si>
+  <si>
+    <t>Erreur inconnue.</t>
+  </si>
+  <si>
+    <t>#3003</t>
+  </si>
+  <si>
+    <t>Impossible de récupérer la correction.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +119,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,11 +170,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,6 +215,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC046F83-2FCC-4DB5-B4F0-E82B9A08A63D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +552,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -514,41 +561,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:A4"/>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Achivement of tests for history & geography
</commit_message>
<xml_diff>
--- a/Error_codes.xlsx
+++ b/Error_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\WampServer\www\learningCenter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8AF8E2-02F8-4E2A-805B-D6B3687F79E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230DB021-8B86-4B1C-8C79-424FEA15F84A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{63368EE7-2865-4327-9FAE-68BBA3F8F765}"/>
+    <workbookView xWindow="2655" yWindow="1410" windowWidth="16200" windowHeight="9360" xr2:uid="{63368EE7-2865-4327-9FAE-68BBA3F8F765}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Code</t>
   </si>
@@ -68,26 +68,38 @@
     <t>#3001</t>
   </si>
   <si>
-    <t>Non trouvé
+    <t>#1000</t>
+  </si>
+  <si>
+    <t>Fichier non trouvé.</t>
+  </si>
+  <si>
+    <t>#3002</t>
+  </si>
+  <si>
+    <t>Erreur inconnue.</t>
+  </si>
+  <si>
+    <t>#3003</t>
+  </si>
+  <si>
+    <t>Impossible de récupérer la correction.</t>
+  </si>
+  <si>
+    <t>#3004</t>
+  </si>
+  <si>
+    <t>Impossible de récupérer les données du test.</t>
+  </si>
+  <si>
+    <t>Générique
 #1</t>
   </si>
   <si>
-    <t>#1000</t>
-  </si>
-  <si>
-    <t>Fichier non trouvé.</t>
-  </si>
-  <si>
-    <t>#3002</t>
-  </si>
-  <si>
-    <t>Erreur inconnue.</t>
-  </si>
-  <si>
-    <t>#3003</t>
-  </si>
-  <si>
-    <t>Impossible de récupérer la correction.</t>
+    <t>#1002</t>
+  </si>
+  <si>
+    <t>Erreur lors de la lecture de la ressource.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -183,11 +195,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,6 +243,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC046F83-2FCC-4DB5-B4F0-E82B9A08A63D}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,68 +589,86 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>